<commit_message>
spixconv: Single ioc per container
</commit_message>
<xml_diff>
--- a/scripts/spreadsheet/SPIxCONV.xlsx
+++ b/scripts/spreadsheet/SPIxCONV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1264\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18DC2CE6-C703-4DE7-AC77-D66CDB7A284D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{056C5D9C-B95D-47B4-98D6-4DD90A402BBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1200,7 +1201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1352,6 +1353,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1359,6 +1363,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1400,46 +1437,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1769,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AO33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8:M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1812,142 +1816,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" ht="15" customHeight="1">
-      <c r="B1" s="50"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="67" t="s">
+      <c r="S1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="69"/>
-      <c r="V1" s="70" t="s">
+      <c r="U1" s="79"/>
+      <c r="V1" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="70" t="s">
+      <c r="W1" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="56" t="s">
+      <c r="X1" s="51"/>
+      <c r="Y1" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="50"/>
-      <c r="AH1" s="54" t="s">
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="50"/>
-      <c r="AJ1" s="50"/>
-      <c r="AK1" s="50"/>
-      <c r="AM1" s="50"/>
-      <c r="AN1" s="50"/>
-      <c r="AO1" s="50"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
     </row>
     <row r="2" spans="2:41">
-      <c r="B2" s="50"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
       <c r="T2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50" t="s">
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="AE2" s="50" t="s">
+      <c r="AE2" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="50" t="s">
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="50"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="51"/>
       <c r="AJ2" s="44" t="s">
         <v>27</v>
       </c>
       <c r="AK2" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AM2" s="50"/>
+      <c r="AM2" s="51"/>
       <c r="AN2" s="44" t="s">
         <v>27</v>
       </c>
@@ -1956,7 +1960,7 @@
       </c>
     </row>
     <row r="3" spans="2:41" ht="30">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2024,46 +2028,46 @@
       <c r="W3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="51">
+      <c r="X3" s="51"/>
+      <c r="Y3" s="52">
         <v>10</v>
       </c>
-      <c r="Z3" s="50">
+      <c r="Z3" s="51">
         <v>128</v>
       </c>
-      <c r="AA3" s="50">
+      <c r="AA3" s="51">
         <v>170</v>
       </c>
-      <c r="AB3" s="52">
+      <c r="AB3" s="53">
         <v>107</v>
       </c>
-      <c r="AC3" s="50"/>
-      <c r="AD3" s="50" t="s">
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE3" s="50" t="s">
+      <c r="AE3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF3" s="50" t="s">
+      <c r="AF3" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG3" s="50" t="s">
+      <c r="AG3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH3" s="50"/>
-      <c r="AI3" s="50"/>
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51"/>
       <c r="AJ3" s="42">
         <v>1</v>
       </c>
       <c r="AK3" s="46"/>
-      <c r="AM3" s="50"/>
+      <c r="AM3" s="51"/>
       <c r="AN3" s="42">
         <v>21</v>
       </c>
       <c r="AO3" s="46"/>
     </row>
     <row r="4" spans="2:41" ht="30">
-      <c r="B4" s="72"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
@@ -2130,34 +2134,34 @@
       <c r="W4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="51">
+      <c r="X4" s="51"/>
+      <c r="Y4" s="52">
         <v>10</v>
       </c>
-      <c r="Z4" s="50">
+      <c r="Z4" s="51">
         <v>128</v>
       </c>
-      <c r="AA4" s="50">
+      <c r="AA4" s="51">
         <v>170</v>
       </c>
-      <c r="AB4" s="52">
+      <c r="AB4" s="53">
         <v>108</v>
       </c>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50" t="s">
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE4" s="50" t="s">
+      <c r="AE4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF4" s="50" t="s">
+      <c r="AF4" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG4" s="50" t="s">
+      <c r="AG4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
+      <c r="AH4" s="51"/>
+      <c r="AI4" s="51"/>
       <c r="AJ4" s="42">
         <v>2</v>
       </c>
@@ -2167,14 +2171,14 @@
       <c r="AL4" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="AM4" s="50"/>
+      <c r="AM4" s="51"/>
       <c r="AN4" s="42">
         <v>22</v>
       </c>
       <c r="AO4" s="46"/>
     </row>
     <row r="5" spans="2:41" ht="30">
-      <c r="B5" s="72"/>
+      <c r="B5" s="81"/>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
@@ -2241,34 +2245,34 @@
       <c r="W5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="51">
+      <c r="X5" s="51"/>
+      <c r="Y5" s="52">
         <v>10</v>
       </c>
-      <c r="Z5" s="50">
+      <c r="Z5" s="51">
         <v>128</v>
       </c>
-      <c r="AA5" s="50">
+      <c r="AA5" s="51">
         <v>170</v>
       </c>
-      <c r="AB5" s="52">
+      <c r="AB5" s="53">
         <v>109</v>
       </c>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="50" t="s">
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE5" s="50" t="s">
+      <c r="AE5" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF5" s="50" t="s">
+      <c r="AF5" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG5" s="50" t="s">
+      <c r="AG5" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH5" s="50"/>
-      <c r="AI5" s="50"/>
+      <c r="AH5" s="51"/>
+      <c r="AI5" s="51"/>
       <c r="AJ5" s="42">
         <v>3</v>
       </c>
@@ -2278,14 +2282,14 @@
       <c r="AL5" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="AM5" s="50"/>
+      <c r="AM5" s="51"/>
       <c r="AN5" s="42">
         <v>23</v>
       </c>
       <c r="AO5" s="46"/>
     </row>
     <row r="6" spans="2:41" ht="30">
-      <c r="B6" s="72"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
@@ -2352,34 +2356,34 @@
       <c r="W6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="X6" s="50"/>
-      <c r="Y6" s="51">
+      <c r="X6" s="51"/>
+      <c r="Y6" s="52">
         <v>10</v>
       </c>
-      <c r="Z6" s="50">
+      <c r="Z6" s="51">
         <v>128</v>
       </c>
-      <c r="AA6" s="50">
+      <c r="AA6" s="51">
         <v>170</v>
       </c>
-      <c r="AB6" s="52">
+      <c r="AB6" s="53">
         <v>110</v>
       </c>
-      <c r="AC6" s="50"/>
-      <c r="AD6" s="50" t="s">
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE6" s="50" t="s">
+      <c r="AE6" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF6" s="50" t="s">
+      <c r="AF6" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG6" s="50" t="s">
+      <c r="AG6" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH6" s="50"/>
-      <c r="AI6" s="50"/>
+      <c r="AH6" s="51"/>
+      <c r="AI6" s="51"/>
       <c r="AJ6" s="42">
         <v>4</v>
       </c>
@@ -2389,14 +2393,14 @@
       <c r="AL6" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AM6" s="50"/>
+      <c r="AM6" s="51"/>
       <c r="AN6" s="42">
         <v>24</v>
       </c>
       <c r="AO6" s="46"/>
     </row>
     <row r="7" spans="2:41" ht="30">
-      <c r="B7" s="72"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
@@ -2463,34 +2467,34 @@
       <c r="W7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="51">
+      <c r="X7" s="51"/>
+      <c r="Y7" s="52">
         <v>10</v>
       </c>
-      <c r="Z7" s="50">
+      <c r="Z7" s="51">
         <v>128</v>
       </c>
-      <c r="AA7" s="50">
+      <c r="AA7" s="51">
         <v>170</v>
       </c>
-      <c r="AB7" s="52">
+      <c r="AB7" s="53">
         <v>111</v>
       </c>
-      <c r="AC7" s="50"/>
-      <c r="AD7" s="50" t="s">
+      <c r="AC7" s="51"/>
+      <c r="AD7" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE7" s="50" t="s">
+      <c r="AE7" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF7" s="50" t="s">
+      <c r="AF7" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG7" s="50" t="s">
+      <c r="AG7" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH7" s="50"/>
-      <c r="AI7" s="50"/>
+      <c r="AH7" s="51"/>
+      <c r="AI7" s="51"/>
       <c r="AJ7" s="42">
         <v>5</v>
       </c>
@@ -2500,14 +2504,14 @@
       <c r="AL7" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="AM7" s="50"/>
+      <c r="AM7" s="51"/>
       <c r="AN7" s="42">
         <v>25</v>
       </c>
       <c r="AO7" s="46"/>
     </row>
     <row r="8" spans="2:41" ht="18.75">
-      <c r="B8" s="72"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="8" t="s">
         <v>30</v>
       </c>
@@ -2541,7 +2545,7 @@
       <c r="L8" s="10">
         <v>88</v>
       </c>
-      <c r="M8" s="77">
+      <c r="M8" s="55">
         <v>88</v>
       </c>
       <c r="N8" s="9" t="s">
@@ -2572,32 +2576,32 @@
       <c r="W8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="51">
+      <c r="X8" s="51"/>
+      <c r="Y8" s="52">
         <v>10</v>
       </c>
-      <c r="Z8" s="50">
+      <c r="Z8" s="51">
         <v>128</v>
       </c>
-      <c r="AA8" s="50">
+      <c r="AA8" s="51">
         <v>170</v>
       </c>
-      <c r="AB8" s="52">
+      <c r="AB8" s="53">
         <v>112</v>
       </c>
-      <c r="AC8" s="50"/>
-      <c r="AD8" s="50" t="s">
+      <c r="AC8" s="51"/>
+      <c r="AD8" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AE8" s="50" t="s">
+      <c r="AE8" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AF8" s="50"/>
-      <c r="AG8" s="50" t="s">
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH8" s="50"/>
-      <c r="AI8" s="50"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
       <c r="AJ8" s="42">
         <v>6</v>
       </c>
@@ -2607,14 +2611,14 @@
       <c r="AL8" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="AM8" s="50"/>
+      <c r="AM8" s="51"/>
       <c r="AN8" s="42">
         <v>26</v>
       </c>
       <c r="AO8" s="46"/>
     </row>
     <row r="9" spans="2:41" ht="18.75">
-      <c r="B9" s="72"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="12" t="s">
         <v>30</v>
       </c>
@@ -2648,7 +2652,7 @@
       <c r="L9" s="14">
         <v>8</v>
       </c>
-      <c r="M9" s="78">
+      <c r="M9" s="56">
         <v>88</v>
       </c>
       <c r="N9" s="13" t="s">
@@ -2681,34 +2685,34 @@
       <c r="W9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="51">
+      <c r="X9" s="51"/>
+      <c r="Y9" s="52">
         <v>10</v>
       </c>
-      <c r="Z9" s="50">
+      <c r="Z9" s="51">
         <v>128</v>
       </c>
-      <c r="AA9" s="50">
+      <c r="AA9" s="51">
         <v>170</v>
       </c>
-      <c r="AB9" s="52">
+      <c r="AB9" s="53">
         <v>113</v>
       </c>
-      <c r="AC9" s="50"/>
-      <c r="AD9" s="50" t="s">
+      <c r="AC9" s="51"/>
+      <c r="AD9" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE9" s="50" t="s">
+      <c r="AE9" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF9" s="50" t="s">
+      <c r="AF9" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG9" s="50" t="s">
+      <c r="AG9" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH9" s="50"/>
-      <c r="AI9" s="50"/>
+      <c r="AH9" s="51"/>
+      <c r="AI9" s="51"/>
       <c r="AJ9" s="42">
         <v>7</v>
       </c>
@@ -2718,14 +2722,14 @@
       <c r="AL9" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="AM9" s="50"/>
+      <c r="AM9" s="51"/>
       <c r="AN9" s="42">
         <v>27</v>
       </c>
       <c r="AO9" s="46"/>
     </row>
     <row r="10" spans="2:41" ht="30">
-      <c r="B10" s="72"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="16" t="s">
         <v>30</v>
       </c>
@@ -2759,7 +2763,7 @@
       <c r="L10" s="4">
         <v>2</v>
       </c>
-      <c r="M10" s="79">
+      <c r="M10" s="57">
         <v>88</v>
       </c>
       <c r="N10" s="4" t="s">
@@ -2792,34 +2796,34 @@
       <c r="W10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="X10" s="50"/>
-      <c r="Y10" s="51">
+      <c r="X10" s="51"/>
+      <c r="Y10" s="52">
         <v>10</v>
       </c>
-      <c r="Z10" s="50">
+      <c r="Z10" s="51">
         <v>128</v>
       </c>
-      <c r="AA10" s="50">
+      <c r="AA10" s="51">
         <v>180</v>
       </c>
-      <c r="AB10" s="52">
+      <c r="AB10" s="53">
         <v>107</v>
       </c>
-      <c r="AC10" s="50"/>
-      <c r="AD10" s="50" t="s">
+      <c r="AC10" s="51"/>
+      <c r="AD10" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE10" s="50" t="s">
+      <c r="AE10" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF10" s="50" t="s">
+      <c r="AF10" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG10" s="50" t="s">
+      <c r="AG10" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH10" s="50"/>
-      <c r="AI10" s="50"/>
+      <c r="AH10" s="51"/>
+      <c r="AI10" s="51"/>
       <c r="AJ10" s="42">
         <v>8</v>
       </c>
@@ -2829,14 +2833,14 @@
       <c r="AL10" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="AM10" s="50"/>
+      <c r="AM10" s="51"/>
       <c r="AN10" s="42">
         <v>28</v>
       </c>
       <c r="AO10" s="46"/>
     </row>
     <row r="11" spans="2:41" ht="45">
-      <c r="B11" s="72"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
@@ -2870,7 +2874,7 @@
       <c r="L11" s="4">
         <v>9</v>
       </c>
-      <c r="M11" s="80">
+      <c r="M11" s="58">
         <v>88</v>
       </c>
       <c r="N11" s="6" t="s">
@@ -2903,34 +2907,34 @@
       <c r="W11" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="51">
+      <c r="X11" s="51"/>
+      <c r="Y11" s="52">
         <v>10</v>
       </c>
-      <c r="Z11" s="50">
+      <c r="Z11" s="51">
         <v>128</v>
       </c>
-      <c r="AA11" s="50">
+      <c r="AA11" s="51">
         <v>180</v>
       </c>
-      <c r="AB11" s="52">
+      <c r="AB11" s="53">
         <v>108</v>
       </c>
-      <c r="AC11" s="50"/>
-      <c r="AD11" s="50" t="s">
+      <c r="AC11" s="51"/>
+      <c r="AD11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE11" s="50" t="s">
+      <c r="AE11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF11" s="50" t="s">
+      <c r="AF11" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG11" s="50" t="s">
+      <c r="AG11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH11" s="50"/>
-      <c r="AI11" s="50"/>
+      <c r="AH11" s="51"/>
+      <c r="AI11" s="51"/>
       <c r="AJ11" s="42">
         <v>9</v>
       </c>
@@ -2940,14 +2944,14 @@
       <c r="AL11" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="AM11" s="50"/>
+      <c r="AM11" s="51"/>
       <c r="AN11" s="42">
         <v>29</v>
       </c>
       <c r="AO11" s="46"/>
     </row>
     <row r="12" spans="2:41" ht="45">
-      <c r="B12" s="72"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
@@ -2981,7 +2985,7 @@
       <c r="L12" s="4">
         <v>6</v>
       </c>
-      <c r="M12" s="80">
+      <c r="M12" s="58">
         <v>88</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -3014,34 +3018,34 @@
       <c r="W12" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="51">
+      <c r="X12" s="51"/>
+      <c r="Y12" s="52">
         <v>10</v>
       </c>
-      <c r="Z12" s="50">
+      <c r="Z12" s="51">
         <v>128</v>
       </c>
-      <c r="AA12" s="50">
+      <c r="AA12" s="51">
         <v>180</v>
       </c>
-      <c r="AB12" s="52">
+      <c r="AB12" s="53">
         <v>109</v>
       </c>
-      <c r="AC12" s="50"/>
-      <c r="AD12" s="50" t="s">
+      <c r="AC12" s="51"/>
+      <c r="AD12" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE12" s="50" t="s">
+      <c r="AE12" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF12" s="50" t="s">
+      <c r="AF12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG12" s="50" t="s">
+      <c r="AG12" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH12" s="50"/>
-      <c r="AI12" s="50"/>
+      <c r="AH12" s="51"/>
+      <c r="AI12" s="51"/>
       <c r="AJ12" s="42">
         <v>10</v>
       </c>
@@ -3051,14 +3055,14 @@
       <c r="AL12" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="AM12" s="50"/>
+      <c r="AM12" s="51"/>
       <c r="AN12" s="42">
         <v>30</v>
       </c>
       <c r="AO12" s="46"/>
     </row>
     <row r="13" spans="2:41" ht="18.75">
-      <c r="B13" s="72"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="12" t="s">
         <v>30</v>
       </c>
@@ -3073,11 +3077,11 @@
         <v>124</v>
       </c>
       <c r="G13" s="13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="13">
         <v>8000</v>
@@ -3092,7 +3096,7 @@
       <c r="L13" s="17">
         <v>88</v>
       </c>
-      <c r="M13" s="78">
+      <c r="M13" s="56">
         <v>88</v>
       </c>
       <c r="N13" s="13" t="s">
@@ -3125,46 +3129,46 @@
       <c r="W13" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="51">
+      <c r="X13" s="51"/>
+      <c r="Y13" s="52">
         <v>10</v>
       </c>
-      <c r="Z13" s="50">
+      <c r="Z13" s="51">
         <v>128</v>
       </c>
-      <c r="AA13" s="50">
+      <c r="AA13" s="51">
         <v>180</v>
       </c>
-      <c r="AB13" s="52">
+      <c r="AB13" s="53">
         <v>110</v>
       </c>
-      <c r="AC13" s="50"/>
-      <c r="AD13" s="50" t="s">
+      <c r="AC13" s="51"/>
+      <c r="AD13" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AE13" s="50" t="s">
+      <c r="AE13" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF13" s="50" t="s">
+      <c r="AF13" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG13" s="50" t="s">
+      <c r="AG13" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH13" s="50"/>
-      <c r="AI13" s="50"/>
+      <c r="AH13" s="51"/>
+      <c r="AI13" s="51"/>
       <c r="AJ13" s="42">
         <v>11</v>
       </c>
       <c r="AK13" s="46"/>
-      <c r="AM13" s="50"/>
+      <c r="AM13" s="51"/>
       <c r="AN13" s="42">
         <v>31</v>
       </c>
       <c r="AO13" s="46"/>
     </row>
     <row r="14" spans="2:41" ht="18.75">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="72" t="s">
         <v>127</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -3200,7 +3204,7 @@
       <c r="L14" s="4">
         <v>1</v>
       </c>
-      <c r="M14" s="79">
+      <c r="M14" s="57">
         <v>88</v>
       </c>
       <c r="N14" s="4" t="s">
@@ -3227,44 +3231,44 @@
       <c r="W14" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="X14" s="50"/>
-      <c r="Y14" s="51">
+      <c r="X14" s="51"/>
+      <c r="Y14" s="52">
         <v>10</v>
       </c>
-      <c r="Z14" s="50">
+      <c r="Z14" s="51">
         <v>128</v>
       </c>
-      <c r="AA14" s="50">
+      <c r="AA14" s="51">
         <v>170</v>
       </c>
-      <c r="AB14" s="52">
+      <c r="AB14" s="53">
         <v>114</v>
       </c>
-      <c r="AC14" s="50"/>
-      <c r="AD14" s="50"/>
-      <c r="AE14" s="50" t="s">
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF14" s="50" t="s">
+      <c r="AF14" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG14" s="50" t="s">
+      <c r="AG14" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH14" s="50"/>
-      <c r="AI14" s="50"/>
+      <c r="AH14" s="51"/>
+      <c r="AI14" s="51"/>
       <c r="AJ14" s="42">
         <v>12</v>
       </c>
       <c r="AK14" s="46"/>
-      <c r="AM14" s="50"/>
+      <c r="AM14" s="51"/>
       <c r="AN14" s="42">
         <v>32</v>
       </c>
       <c r="AO14" s="46"/>
     </row>
     <row r="15" spans="2:41" ht="18.75">
-      <c r="B15" s="60"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="19" t="s">
         <v>30</v>
       </c>
@@ -3298,7 +3302,7 @@
       <c r="L15" s="4">
         <v>3</v>
       </c>
-      <c r="M15" s="80">
+      <c r="M15" s="58">
         <v>88</v>
       </c>
       <c r="N15" s="6" t="s">
@@ -3325,34 +3329,34 @@
       <c r="W15" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="51">
+      <c r="X15" s="51"/>
+      <c r="Y15" s="52">
         <v>10</v>
       </c>
-      <c r="Z15" s="50">
+      <c r="Z15" s="51">
         <v>128</v>
       </c>
-      <c r="AA15" s="50">
+      <c r="AA15" s="51">
         <v>180</v>
       </c>
-      <c r="AB15" s="52">
+      <c r="AB15" s="53">
         <v>111</v>
       </c>
-      <c r="AC15" s="50"/>
-      <c r="AD15" s="50" t="s">
+      <c r="AC15" s="51"/>
+      <c r="AD15" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE15" s="50" t="s">
+      <c r="AE15" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="AF15" s="50" t="s">
+      <c r="AF15" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG15" s="50" t="s">
+      <c r="AG15" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH15" s="50"/>
-      <c r="AI15" s="50"/>
+      <c r="AH15" s="51"/>
+      <c r="AI15" s="51"/>
       <c r="AJ15" s="42">
         <v>13</v>
       </c>
@@ -3362,14 +3366,14 @@
       <c r="AL15" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="AM15" s="50"/>
+      <c r="AM15" s="51"/>
       <c r="AN15" s="42">
         <v>33</v>
       </c>
       <c r="AO15" s="46"/>
     </row>
     <row r="16" spans="2:41" ht="18.75">
-      <c r="B16" s="60"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="19" t="s">
         <v>140</v>
       </c>
@@ -3402,7 +3406,7 @@
       <c r="L16" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="M16" s="80">
+      <c r="M16" s="58">
         <v>88</v>
       </c>
       <c r="N16" s="6" t="s">
@@ -3429,34 +3433,34 @@
       <c r="W16" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="61" t="s">
+      <c r="X16" s="51"/>
+      <c r="Y16" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="Z16" s="62"/>
-      <c r="AA16" s="62"/>
-      <c r="AB16" s="63"/>
-      <c r="AC16" s="50"/>
-      <c r="AD16" s="50"/>
-      <c r="AE16" s="50" t="s">
+      <c r="Z16" s="74"/>
+      <c r="AA16" s="74"/>
+      <c r="AB16" s="75"/>
+      <c r="AC16" s="51"/>
+      <c r="AD16" s="51"/>
+      <c r="AE16" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AF16" s="50"/>
-      <c r="AG16" s="50"/>
-      <c r="AH16" s="50"/>
-      <c r="AI16" s="50"/>
+      <c r="AF16" s="51"/>
+      <c r="AG16" s="51"/>
+      <c r="AH16" s="51"/>
+      <c r="AI16" s="51"/>
       <c r="AJ16" s="42">
         <v>14</v>
       </c>
       <c r="AK16" s="46"/>
-      <c r="AM16" s="50"/>
+      <c r="AM16" s="51"/>
       <c r="AN16" s="42">
         <v>34</v>
       </c>
       <c r="AO16" s="46"/>
     </row>
     <row r="17" spans="2:41" ht="18.75">
-      <c r="B17" s="60"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="19" t="s">
         <v>30</v>
       </c>
@@ -3490,7 +3494,7 @@
       <c r="L17" s="4">
         <v>11</v>
       </c>
-      <c r="M17" s="80">
+      <c r="M17" s="58">
         <v>88</v>
       </c>
       <c r="N17" s="6" t="s">
@@ -3517,46 +3521,46 @@
       <c r="W17" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X17" s="50"/>
-      <c r="Y17" s="51">
+      <c r="X17" s="51"/>
+      <c r="Y17" s="52">
         <v>10</v>
       </c>
-      <c r="Z17" s="50">
+      <c r="Z17" s="51">
         <v>128</v>
       </c>
-      <c r="AA17" s="50">
+      <c r="AA17" s="51">
         <v>170</v>
       </c>
-      <c r="AB17" s="52">
+      <c r="AB17" s="53">
         <v>115</v>
       </c>
-      <c r="AC17" s="50"/>
-      <c r="AD17" s="50" t="s">
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE17" s="50" t="s">
+      <c r="AE17" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AF17" s="50" t="s">
+      <c r="AF17" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG17" s="50" t="s">
+      <c r="AG17" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH17" s="50"/>
-      <c r="AI17" s="50"/>
+      <c r="AH17" s="51"/>
+      <c r="AI17" s="51"/>
       <c r="AJ17" s="42">
         <v>15</v>
       </c>
       <c r="AK17" s="46"/>
-      <c r="AM17" s="50"/>
+      <c r="AM17" s="51"/>
       <c r="AN17" s="42">
         <v>35</v>
       </c>
       <c r="AO17" s="46"/>
     </row>
     <row r="18" spans="2:41" ht="18.75">
-      <c r="B18" s="60"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="19" t="s">
         <v>30</v>
       </c>
@@ -3590,7 +3594,7 @@
       <c r="L18" s="4">
         <v>16</v>
       </c>
-      <c r="M18" s="80">
+      <c r="M18" s="58">
         <v>88</v>
       </c>
       <c r="N18" s="6" t="s">
@@ -3619,42 +3623,42 @@
       <c r="W18" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X18" s="50"/>
-      <c r="Y18" s="51">
+      <c r="X18" s="51"/>
+      <c r="Y18" s="52">
         <v>10</v>
       </c>
-      <c r="Z18" s="50">
+      <c r="Z18" s="51">
         <v>128</v>
       </c>
-      <c r="AA18" s="50">
+      <c r="AA18" s="51">
         <v>180</v>
       </c>
-      <c r="AB18" s="52">
+      <c r="AB18" s="53">
         <v>112</v>
       </c>
-      <c r="AC18" s="50"/>
-      <c r="AD18" s="50"/>
-      <c r="AE18" s="50" t="s">
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="AF18" s="50" t="s">
+      <c r="AF18" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG18" s="50"/>
-      <c r="AH18" s="50"/>
-      <c r="AI18" s="50"/>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="51"/>
+      <c r="AI18" s="51"/>
       <c r="AJ18" s="42">
         <v>16</v>
       </c>
       <c r="AK18" s="46"/>
-      <c r="AM18" s="50"/>
+      <c r="AM18" s="51"/>
       <c r="AN18" s="42">
         <v>36</v>
       </c>
       <c r="AO18" s="46"/>
     </row>
     <row r="19" spans="2:41" ht="18.75">
-      <c r="B19" s="60"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="19" t="s">
         <v>140</v>
       </c>
@@ -3687,7 +3691,7 @@
       <c r="L19" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="M19" s="80">
+      <c r="M19" s="58">
         <v>88</v>
       </c>
       <c r="N19" s="6" t="s">
@@ -3714,22 +3718,22 @@
       <c r="W19" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X19" s="50"/>
-      <c r="Y19" s="61" t="s">
+      <c r="X19" s="51"/>
+      <c r="Y19" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="Z19" s="62"/>
-      <c r="AA19" s="62"/>
-      <c r="AB19" s="63"/>
-      <c r="AC19" s="50"/>
-      <c r="AD19" s="50"/>
-      <c r="AE19" s="50" t="s">
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="74"/>
+      <c r="AB19" s="75"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AF19" s="50"/>
-      <c r="AG19" s="50"/>
-      <c r="AH19" s="50"/>
-      <c r="AI19" s="50"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="51"/>
+      <c r="AI19" s="51"/>
       <c r="AJ19" s="42">
         <v>17</v>
       </c>
@@ -3739,14 +3743,14 @@
       <c r="AL19" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="AM19" s="50"/>
+      <c r="AM19" s="51"/>
       <c r="AN19" s="42">
         <v>37</v>
       </c>
       <c r="AO19" s="46"/>
     </row>
     <row r="20" spans="2:41" ht="18.75">
-      <c r="B20" s="60"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="23" t="s">
         <v>30</v>
       </c>
@@ -3780,7 +3784,7 @@
       <c r="L20" s="25">
         <v>13</v>
       </c>
-      <c r="M20" s="77">
+      <c r="M20" s="55">
         <v>88</v>
       </c>
       <c r="N20" s="9" t="s">
@@ -3813,46 +3817,46 @@
       <c r="W20" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="51">
+      <c r="X20" s="51"/>
+      <c r="Y20" s="52">
         <v>10</v>
       </c>
-      <c r="Z20" s="50">
+      <c r="Z20" s="51">
         <v>128</v>
       </c>
-      <c r="AA20" s="50">
+      <c r="AA20" s="51">
         <v>170</v>
       </c>
-      <c r="AB20" s="52">
+      <c r="AB20" s="53">
         <v>116</v>
       </c>
-      <c r="AC20" s="50"/>
-      <c r="AD20" s="50" t="s">
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AE20" s="50" t="s">
+      <c r="AE20" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="AF20" s="50" t="s">
+      <c r="AF20" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG20" s="50" t="s">
+      <c r="AG20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AH20" s="50"/>
-      <c r="AI20" s="50"/>
+      <c r="AH20" s="51"/>
+      <c r="AI20" s="51"/>
       <c r="AJ20" s="42">
         <v>18</v>
       </c>
       <c r="AK20" s="46"/>
-      <c r="AM20" s="50"/>
+      <c r="AM20" s="51"/>
       <c r="AN20" s="42">
         <v>38</v>
       </c>
       <c r="AO20" s="46"/>
     </row>
     <row r="21" spans="2:41" ht="18.75">
-      <c r="B21" s="60"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="8" t="s">
         <v>140</v>
       </c>
@@ -3885,7 +3889,7 @@
       <c r="L21" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="M21" s="80">
+      <c r="M21" s="58">
         <v>88</v>
       </c>
       <c r="N21" s="9" t="s">
@@ -3912,34 +3916,34 @@
       <c r="W21" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="61" t="s">
+      <c r="X21" s="51"/>
+      <c r="Y21" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="Z21" s="62"/>
-      <c r="AA21" s="62"/>
-      <c r="AB21" s="63"/>
-      <c r="AC21" s="50"/>
-      <c r="AD21" s="50"/>
-      <c r="AE21" s="50" t="s">
+      <c r="Z21" s="74"/>
+      <c r="AA21" s="74"/>
+      <c r="AB21" s="75"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AF21" s="50"/>
-      <c r="AG21" s="50"/>
-      <c r="AH21" s="50"/>
-      <c r="AI21" s="50"/>
+      <c r="AF21" s="51"/>
+      <c r="AG21" s="51"/>
+      <c r="AH21" s="51"/>
+      <c r="AI21" s="51"/>
       <c r="AJ21" s="42">
         <v>19</v>
       </c>
       <c r="AK21" s="46"/>
-      <c r="AM21" s="50"/>
+      <c r="AM21" s="51"/>
       <c r="AN21" s="42">
         <v>39</v>
       </c>
       <c r="AO21" s="46"/>
     </row>
     <row r="22" spans="2:41" ht="18.75">
-      <c r="B22" s="60"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="3" t="s">
         <v>140</v>
       </c>
@@ -3999,36 +4003,36 @@
       <c r="W22" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="X22" s="50"/>
-      <c r="Y22" s="64" t="s">
+      <c r="X22" s="51"/>
+      <c r="Y22" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="Z22" s="65"/>
-      <c r="AA22" s="65"/>
-      <c r="AB22" s="66"/>
-      <c r="AC22" s="50"/>
-      <c r="AD22" s="50"/>
-      <c r="AE22" s="50" t="s">
+      <c r="Z22" s="77"/>
+      <c r="AA22" s="77"/>
+      <c r="AB22" s="78"/>
+      <c r="AC22" s="51"/>
+      <c r="AD22" s="51"/>
+      <c r="AE22" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="AF22" s="50" t="s">
+      <c r="AF22" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG22" s="50"/>
-      <c r="AH22" s="50"/>
-      <c r="AI22" s="50"/>
+      <c r="AG22" s="51"/>
+      <c r="AH22" s="51"/>
+      <c r="AI22" s="51"/>
       <c r="AJ22" s="43">
         <v>20</v>
       </c>
       <c r="AK22" s="47"/>
-      <c r="AM22" s="50"/>
+      <c r="AM22" s="51"/>
       <c r="AN22" s="43">
         <v>40</v>
       </c>
       <c r="AO22" s="47"/>
     </row>
     <row r="23" spans="2:41" ht="18.75">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="54" t="s">
         <v>171</v>
       </c>
       <c r="C23" s="28" t="s">
@@ -4089,7 +4093,7 @@
       <c r="W23" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="X23" s="50"/>
+      <c r="X23" s="51"/>
       <c r="Y23" s="36">
         <v>10</v>
       </c>
@@ -4102,373 +4106,368 @@
       <c r="AB23" s="37">
         <v>40</v>
       </c>
-      <c r="AC23" s="50"/>
-      <c r="AD23" s="50"/>
-      <c r="AE23" s="50" t="s">
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="AF23" s="50" t="s">
+      <c r="AF23" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AG23" s="50"/>
-      <c r="AH23" s="50"/>
-      <c r="AI23" s="50"/>
-      <c r="AJ23" s="50"/>
-      <c r="AK23" s="50"/>
-      <c r="AM23" s="50"/>
-      <c r="AN23" s="50"/>
-      <c r="AO23" s="50"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="51"/>
+      <c r="AI23" s="51"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="51"/>
+      <c r="AM23" s="51"/>
+      <c r="AN23" s="51"/>
+      <c r="AO23" s="51"/>
     </row>
     <row r="25" spans="2:41">
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="50"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-      <c r="T25" s="50"/>
-      <c r="U25" s="50"/>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="50"/>
-      <c r="Z25" s="50"/>
-      <c r="AA25" s="50"/>
-      <c r="AB25" s="50"/>
-      <c r="AC25" s="50"/>
-      <c r="AD25" s="50"/>
-      <c r="AE25" s="50"/>
-      <c r="AF25" s="50" t="s">
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="51"/>
+      <c r="W25" s="51"/>
+      <c r="X25" s="51"/>
+      <c r="Y25" s="51"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="51"/>
+      <c r="AB25" s="51"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+      <c r="AE25" s="51"/>
+      <c r="AF25" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="AG25" s="50"/>
-      <c r="AH25" s="50"/>
-      <c r="AI25" s="50"/>
-      <c r="AJ25" s="50"/>
-      <c r="AK25" s="50"/>
-      <c r="AM25" s="50"/>
-      <c r="AN25" s="50"/>
-      <c r="AO25" s="50"/>
+      <c r="AG25" s="51"/>
+      <c r="AH25" s="51"/>
+      <c r="AI25" s="51"/>
+      <c r="AJ25" s="51"/>
+      <c r="AK25" s="51"/>
+      <c r="AM25" s="51"/>
+      <c r="AN25" s="51"/>
+      <c r="AO25" s="51"/>
     </row>
     <row r="27" spans="2:41">
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
       <c r="M27" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="N27" s="50" t="s">
+      <c r="N27" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
       <c r="T27" s="39"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="50"/>
-      <c r="Z27" s="50"/>
-      <c r="AA27" s="50"/>
-      <c r="AB27" s="50"/>
-      <c r="AC27" s="50"/>
-      <c r="AD27" s="50"/>
-      <c r="AE27" s="50"/>
-      <c r="AF27" s="50"/>
-      <c r="AG27" s="50"/>
-      <c r="AH27" s="50"/>
-      <c r="AI27" s="50"/>
-      <c r="AJ27" s="50"/>
-      <c r="AK27" s="50"/>
-      <c r="AM27" s="50"/>
-      <c r="AN27" s="50"/>
-      <c r="AO27" s="50"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="51"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="51"/>
+      <c r="AG27" s="51"/>
+      <c r="AH27" s="51"/>
+      <c r="AI27" s="51"/>
+      <c r="AJ27" s="51"/>
+      <c r="AK27" s="51"/>
+      <c r="AM27" s="51"/>
+      <c r="AN27" s="51"/>
+      <c r="AO27" s="51"/>
     </row>
     <row r="28" spans="2:41">
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
       <c r="T28" s="39"/>
-      <c r="U28" s="50"/>
-      <c r="V28" s="50"/>
-      <c r="W28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="50"/>
-      <c r="Z28" s="50"/>
-      <c r="AA28" s="50"/>
-      <c r="AB28" s="50"/>
-      <c r="AC28" s="50"/>
-      <c r="AD28" s="50"/>
-      <c r="AE28" s="50"/>
-      <c r="AF28" s="50"/>
-      <c r="AG28" s="50"/>
-      <c r="AH28" s="50"/>
-      <c r="AI28" s="50"/>
-      <c r="AJ28" s="50"/>
-      <c r="AK28" s="50"/>
-      <c r="AM28" s="50"/>
-      <c r="AN28" s="50"/>
-      <c r="AO28" s="50"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
+      <c r="Y28" s="51"/>
+      <c r="Z28" s="51"/>
+      <c r="AA28" s="51"/>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="51"/>
+      <c r="AF28" s="51"/>
+      <c r="AG28" s="51"/>
+      <c r="AH28" s="51"/>
+      <c r="AI28" s="51"/>
+      <c r="AJ28" s="51"/>
+      <c r="AK28" s="51"/>
+      <c r="AM28" s="51"/>
+      <c r="AN28" s="51"/>
+      <c r="AO28" s="51"/>
     </row>
     <row r="29" spans="2:41">
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="50" t="s">
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="O29" s="50"/>
-      <c r="P29" s="50"/>
-      <c r="Q29" s="50"/>
-      <c r="R29" s="50"/>
-      <c r="S29" s="50"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
       <c r="T29" s="39"/>
-      <c r="U29" s="50"/>
-      <c r="V29" s="50">
+      <c r="U29" s="51"/>
+      <c r="V29" s="51">
         <v>14</v>
       </c>
-      <c r="W29" s="50"/>
-      <c r="X29" s="50"/>
-      <c r="Y29" s="50"/>
-      <c r="Z29" s="50"/>
-      <c r="AA29" s="50"/>
-      <c r="AB29" s="50"/>
-      <c r="AC29" s="50"/>
-      <c r="AD29" s="50"/>
-      <c r="AE29" s="50"/>
-      <c r="AF29" s="50"/>
-      <c r="AG29" s="50"/>
-      <c r="AH29" s="50"/>
-      <c r="AI29" s="50"/>
-      <c r="AJ29" s="50"/>
-      <c r="AK29" s="50"/>
-      <c r="AM29" s="50"/>
-      <c r="AN29" s="50"/>
-      <c r="AO29" s="50"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
+      <c r="Y29" s="51"/>
+      <c r="Z29" s="51"/>
+      <c r="AA29" s="51"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AF29" s="51"/>
+      <c r="AG29" s="51"/>
+      <c r="AH29" s="51"/>
+      <c r="AI29" s="51"/>
+      <c r="AJ29" s="51"/>
+      <c r="AK29" s="51"/>
+      <c r="AM29" s="51"/>
+      <c r="AN29" s="51"/>
+      <c r="AO29" s="51"/>
     </row>
     <row r="30" spans="2:41">
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50" t="s">
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="50"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
       <c r="T30" s="39"/>
-      <c r="U30" s="50"/>
-      <c r="V30" s="50">
+      <c r="U30" s="51"/>
+      <c r="V30" s="51">
         <v>18</v>
       </c>
-      <c r="W30" s="50"/>
-      <c r="X30" s="50"/>
-      <c r="Y30" s="50"/>
-      <c r="Z30" s="50"/>
-      <c r="AA30" s="50"/>
-      <c r="AB30" s="50"/>
-      <c r="AC30" s="50"/>
-      <c r="AD30" s="50"/>
-      <c r="AE30" s="50"/>
-      <c r="AF30" s="50"/>
-      <c r="AG30" s="50"/>
-      <c r="AH30" s="50"/>
-      <c r="AI30" s="50"/>
-      <c r="AJ30" s="50"/>
-      <c r="AK30" s="50"/>
-      <c r="AM30" s="50"/>
-      <c r="AN30" s="50"/>
-      <c r="AO30" s="50"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="51"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="51"/>
+      <c r="AI30" s="51"/>
+      <c r="AJ30" s="51"/>
+      <c r="AK30" s="51"/>
+      <c r="AM30" s="51"/>
+      <c r="AN30" s="51"/>
+      <c r="AO30" s="51"/>
     </row>
     <row r="31" spans="2:41">
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="50"/>
-      <c r="U31" s="50"/>
-      <c r="V31" s="50">
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="51">
         <v>19</v>
       </c>
-      <c r="W31" s="50"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="50"/>
-      <c r="Z31" s="50"/>
-      <c r="AA31" s="50"/>
-      <c r="AB31" s="50"/>
-      <c r="AC31" s="50"/>
-      <c r="AD31" s="50"/>
-      <c r="AE31" s="50"/>
-      <c r="AF31" s="50"/>
-      <c r="AG31" s="50"/>
-      <c r="AH31" s="50"/>
-      <c r="AI31" s="50"/>
-      <c r="AJ31" s="50"/>
-      <c r="AK31" s="50"/>
-      <c r="AM31" s="50"/>
-      <c r="AN31" s="50"/>
-      <c r="AO31" s="50"/>
+      <c r="W31" s="51"/>
+      <c r="X31" s="51"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="51"/>
+      <c r="AA31" s="51"/>
+      <c r="AB31" s="51"/>
+      <c r="AC31" s="51"/>
+      <c r="AD31" s="51"/>
+      <c r="AE31" s="51"/>
+      <c r="AF31" s="51"/>
+      <c r="AG31" s="51"/>
+      <c r="AH31" s="51"/>
+      <c r="AI31" s="51"/>
+      <c r="AJ31" s="51"/>
+      <c r="AK31" s="51"/>
+      <c r="AM31" s="51"/>
+      <c r="AN31" s="51"/>
+      <c r="AO31" s="51"/>
     </row>
     <row r="32" spans="2:41">
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="M32" s="50">
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="51">
         <v>11</v>
       </c>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50" t="s">
+      <c r="N32" s="51"/>
+      <c r="O32" s="51" t="s">
         <v>181</v>
       </c>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="50"/>
-      <c r="U32" s="50"/>
-      <c r="V32" s="50">
+      <c r="P32" s="51"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="51"/>
+      <c r="S32" s="51"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="51"/>
+      <c r="V32" s="51">
         <v>20</v>
       </c>
-      <c r="W32" s="50"/>
-      <c r="X32" s="50"/>
-      <c r="Y32" s="50"/>
-      <c r="Z32" s="50"/>
-      <c r="AA32" s="50"/>
-      <c r="AB32" s="50"/>
-      <c r="AC32" s="50"/>
-      <c r="AD32" s="50"/>
-      <c r="AE32" s="50"/>
-      <c r="AF32" s="50"/>
-      <c r="AG32" s="50"/>
-      <c r="AH32" s="50"/>
-      <c r="AI32" s="50"/>
-      <c r="AJ32" s="50"/>
-      <c r="AK32" s="50"/>
-      <c r="AM32" s="50"/>
-      <c r="AN32" s="50"/>
-      <c r="AO32" s="50"/>
+      <c r="W32" s="51"/>
+      <c r="X32" s="51"/>
+      <c r="Y32" s="51"/>
+      <c r="Z32" s="51"/>
+      <c r="AA32" s="51"/>
+      <c r="AB32" s="51"/>
+      <c r="AC32" s="51"/>
+      <c r="AD32" s="51"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="51"/>
+      <c r="AG32" s="51"/>
+      <c r="AH32" s="51"/>
+      <c r="AI32" s="51"/>
+      <c r="AJ32" s="51"/>
+      <c r="AK32" s="51"/>
+      <c r="AM32" s="51"/>
+      <c r="AN32" s="51"/>
+      <c r="AO32" s="51"/>
     </row>
     <row r="33" spans="13:41">
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="50"/>
-      <c r="U33" s="50"/>
-      <c r="V33" s="50">
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="51">
         <v>15</v>
       </c>
-      <c r="W33" s="50"/>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="50"/>
-      <c r="Z33" s="50"/>
-      <c r="AA33" s="50"/>
-      <c r="AB33" s="50"/>
-      <c r="AC33" s="50"/>
-      <c r="AD33" s="50"/>
-      <c r="AE33" s="50"/>
-      <c r="AF33" s="50"/>
-      <c r="AG33" s="50"/>
-      <c r="AH33" s="50"/>
-      <c r="AI33" s="50"/>
-      <c r="AJ33" s="50"/>
-      <c r="AK33" s="50"/>
-      <c r="AM33" s="50"/>
-      <c r="AN33" s="50"/>
-      <c r="AO33" s="50"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="51"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="51"/>
+      <c r="AB33" s="51"/>
+      <c r="AC33" s="51"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="51"/>
+      <c r="AF33" s="51"/>
+      <c r="AG33" s="51"/>
+      <c r="AH33" s="51"/>
+      <c r="AI33" s="51"/>
+      <c r="AJ33" s="51"/>
+      <c r="AK33" s="51"/>
+      <c r="AM33" s="51"/>
+      <c r="AN33" s="51"/>
+      <c r="AO33" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="Y1:AB2"/>
     <mergeCell ref="B14:B22"/>
@@ -4485,6 +4484,18 @@
     <mergeCell ref="B3:B13"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="C1 C3:C1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -4496,34 +4507,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8">
-      <UserInfo>
-        <DisplayName>Fabio Carlos Arroyo</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Samuel de Souza Moreira</DisplayName>
-        <AccountId>38</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007A7E416D919B234B9674A954BD75FE26" ma:contentTypeVersion="10" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="5e29501042629028b58ca0ea2708fb75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8" xmlns:ns3="dfe0e87d-c18b-4fe8-a38f-f5371de371f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6deaf23babed5926d0459b69a2ea13d3" ns2:_="" ns3:_="">
     <xsd:import namespace="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8"/>
@@ -4726,8 +4709,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8">
+      <UserInfo>
+        <DisplayName>Fabio Carlos Arroyo</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Samuel de Souza Moreira</DisplayName>
+        <AccountId>38</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8508753-15A0-4ABC-BB66-E02BD8158946}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F971D8B-4099-49D4-8764-A7DFC966D5AC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4735,5 +4746,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F971D8B-4099-49D4-8764-A7DFC966D5AC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8508753-15A0-4ABC-BB66-E02BD8158946}"/>
 </file>
</xml_diff>